<commit_message>
modified dash rating data file and testimonialgenerator
</commit_message>
<xml_diff>
--- a/assets/duty_rating.xlsx
+++ b/assets/duty_rating.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/277cafe562d23f36/Streamlit_project/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{66C82524-CC8E-B94B-8B96-B7FF4BEF2589}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="51" documentId="8_{66C82524-CC8E-B94B-8B96-B7FF4BEF2589}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9FB55FBA-D4B1-2B4C-BB3D-1E0AF53782A3}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1800" windowWidth="23620" windowHeight="15360" xr2:uid="{DD687E5F-E8A8-F842-AAA4-0D08685AE85B}"/>
+    <workbookView xWindow="9160" yWindow="2040" windowWidth="23620" windowHeight="15360" xr2:uid="{DD687E5F-E8A8-F842-AAA4-0D08685AE85B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="14">
   <si>
     <t>date</t>
   </si>
@@ -51,6 +51,33 @@
   </si>
   <si>
     <t>bin_rating</t>
+  </si>
+  <si>
+    <t>Odd Monday</t>
+  </si>
+  <si>
+    <t>Odd Tuesday</t>
+  </si>
+  <si>
+    <t>Odd Wednesday</t>
+  </si>
+  <si>
+    <t>Odd Thursday</t>
+  </si>
+  <si>
+    <t>Odd Friday</t>
+  </si>
+  <si>
+    <t>Even Monday</t>
+  </si>
+  <si>
+    <t>Even Wednesday</t>
+  </si>
+  <si>
+    <t>Even Thursday</t>
+  </si>
+  <si>
+    <t>Even Friday</t>
   </si>
 </sst>
 </file>
@@ -86,8 +113,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -422,7 +450,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6E5BEC9-0EBA-944D-96E0-DF6087542F2A}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
@@ -448,23 +476,35 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>45299</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
       <c r="C2">
         <f ca="1">ROUND(RAND()*5,0)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D2">
         <f t="shared" ref="D2:E17" ca="1" si="0">ROUND(RAND()*5,0)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E2">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>45300</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
       <c r="C3">
-        <f t="shared" ref="C3:E26" ca="1" si="1">ROUND(RAND()*5,0)</f>
-        <v>3</v>
+        <f t="shared" ref="C3:E27" ca="1" si="1">ROUND(RAND()*5,0)</f>
+        <v>2</v>
       </c>
       <c r="D3">
         <f t="shared" ca="1" si="0"/>
@@ -472,115 +512,164 @@
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>45301</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
       <c r="C4">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>45302</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
       <c r="C5">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>45303</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
       <c r="C6">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>45306</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
       <c r="C7">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>45308</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
       <c r="C8">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>45309</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
       <c r="C9">
         <f t="shared" ca="1" si="1"/>
         <v>4</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>45310</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
       <c r="C10">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <f>A2+14</f>
+        <v>45313</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
       <c r="C11">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="0"/>
@@ -588,37 +677,58 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <f t="shared" ref="A12:A75" si="2">A3+14</f>
+        <v>45314</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
       <c r="C12">
         <f t="shared" ca="1" si="1"/>
         <v>3</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <f t="shared" si="2"/>
+        <v>45315</v>
+      </c>
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
       <c r="C13">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <f t="shared" si="2"/>
+        <v>45316</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
       <c r="C14">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="0"/>
@@ -630,13 +740,20 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <f t="shared" si="2"/>
+        <v>45317</v>
+      </c>
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
       <c r="C15">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="0"/>
@@ -644,76 +761,118 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <f t="shared" si="2"/>
+        <v>45320</v>
+      </c>
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
       <c r="C16">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <f t="shared" si="2"/>
+        <v>45322</v>
+      </c>
+      <c r="B17" t="s">
+        <v>11</v>
+      </c>
       <c r="C17">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <f t="shared" si="2"/>
+        <v>45323</v>
+      </c>
+      <c r="B18" t="s">
+        <v>12</v>
+      </c>
       <c r="C18">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <f t="shared" si="2"/>
+        <v>45324</v>
+      </c>
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
       <c r="C19">
         <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <f t="shared" si="2"/>
+        <v>45327</v>
+      </c>
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
       <c r="C20">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D20">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E20">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <f t="shared" si="2"/>
+        <v>45328</v>
+      </c>
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
       <c r="C21">
         <f t="shared" ca="1" si="1"/>
         <v>1</v>
@@ -724,27 +883,41 @@
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <f t="shared" si="2"/>
+        <v>45329</v>
+      </c>
+      <c r="B22" t="s">
+        <v>7</v>
+      </c>
       <c r="C22">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D22">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E22">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="3:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <f t="shared" si="2"/>
+        <v>45330</v>
+      </c>
+      <c r="B23" t="s">
+        <v>8</v>
+      </c>
       <c r="C23">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D23">
         <f t="shared" ca="1" si="1"/>
@@ -752,48 +925,1434 @@
       </c>
       <c r="E23">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <f t="shared" si="2"/>
+        <v>45331</v>
+      </c>
+      <c r="B24" t="s">
+        <v>9</v>
+      </c>
       <c r="C24">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D24">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E24">
         <f t="shared" ca="1" si="1"/>
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <f t="shared" si="2"/>
+        <v>45334</v>
+      </c>
+      <c r="B25" t="s">
+        <v>10</v>
+      </c>
       <c r="C25">
         <f t="shared" ca="1" si="1"/>
         <v>2</v>
       </c>
       <c r="D25">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E25">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="3:5" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <f t="shared" si="2"/>
+        <v>45336</v>
+      </c>
+      <c r="B26" t="s">
+        <v>11</v>
+      </c>
       <c r="C26">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D26">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E26">
         <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <f t="shared" si="2"/>
+        <v>45337</v>
+      </c>
+      <c r="B27" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="D27">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="E27">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <f t="shared" si="2"/>
+        <v>45338</v>
+      </c>
+      <c r="B28" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28">
+        <f t="shared" ref="C28:E91" ca="1" si="3">ROUND(RAND()*5,0)</f>
+        <v>3</v>
+      </c>
+      <c r="D28">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="E28">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <f t="shared" si="2"/>
+        <v>45341</v>
+      </c>
+      <c r="B29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="D29">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="E29">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <f t="shared" si="2"/>
+        <v>45342</v>
+      </c>
+      <c r="B30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <f t="shared" ca="1" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="E30">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <f t="shared" si="2"/>
+        <v>45343</v>
+      </c>
+      <c r="B31" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="E31">
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <f t="shared" si="2"/>
+        <v>45344</v>
+      </c>
+      <c r="B32" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="D32">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="E32">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <f t="shared" si="2"/>
+        <v>45345</v>
+      </c>
+      <c r="B33" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E33">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <f t="shared" si="2"/>
+        <v>45348</v>
+      </c>
+      <c r="B34" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D34">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="E34">
+        <f t="shared" ca="1" si="3"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <f t="shared" si="2"/>
+        <v>45350</v>
+      </c>
+      <c r="B35" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35">
+        <f t="shared" ca="1" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="D35">
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="E35">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <f t="shared" si="2"/>
+        <v>45351</v>
+      </c>
+      <c r="B36" t="s">
+        <v>12</v>
+      </c>
+      <c r="C36">
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="D36">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="E36">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <f t="shared" si="2"/>
+        <v>45352</v>
+      </c>
+      <c r="B37" t="s">
+        <v>13</v>
+      </c>
+      <c r="C37">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="D37">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <f t="shared" si="2"/>
+        <v>45355</v>
+      </c>
+      <c r="B38" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38">
+        <f t="shared" ca="1" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="D38">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <f t="shared" si="2"/>
+        <v>45356</v>
+      </c>
+      <c r="B39" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="D39">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <f t="shared" si="2"/>
+        <v>45357</v>
+      </c>
+      <c r="B40" t="s">
+        <v>7</v>
+      </c>
+      <c r="C40">
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="D40">
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="E40">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
+        <f t="shared" si="2"/>
+        <v>45358</v>
+      </c>
+      <c r="B41" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="D41">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
+        <f t="shared" si="2"/>
+        <v>45359</v>
+      </c>
+      <c r="B42" t="s">
+        <v>9</v>
+      </c>
+      <c r="C42">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="D42">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E42">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
+        <f t="shared" si="2"/>
+        <v>45362</v>
+      </c>
+      <c r="B43" t="s">
+        <v>10</v>
+      </c>
+      <c r="C43">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="E43">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <f t="shared" si="2"/>
+        <v>45364</v>
+      </c>
+      <c r="B44" t="s">
+        <v>11</v>
+      </c>
+      <c r="C44">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="D44">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="E44">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
+        <f t="shared" si="2"/>
+        <v>45365</v>
+      </c>
+      <c r="B45" t="s">
+        <v>12</v>
+      </c>
+      <c r="C45">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="D45">
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="E45">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
+        <f t="shared" si="2"/>
+        <v>45366</v>
+      </c>
+      <c r="B46" t="s">
+        <v>13</v>
+      </c>
+      <c r="C46">
+        <f t="shared" ca="1" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="D46">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E46">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
+        <f t="shared" si="2"/>
+        <v>45369</v>
+      </c>
+      <c r="B47" t="s">
+        <v>5</v>
+      </c>
+      <c r="C47">
+        <f t="shared" ca="1" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="D47">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E47">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
+        <f t="shared" si="2"/>
+        <v>45370</v>
+      </c>
+      <c r="B48" t="s">
+        <v>6</v>
+      </c>
+      <c r="C48">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="E48">
+        <f t="shared" ca="1" si="3"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
+        <f t="shared" si="2"/>
+        <v>45371</v>
+      </c>
+      <c r="B49" t="s">
+        <v>7</v>
+      </c>
+      <c r="C49">
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="D49">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="E49">
+        <f t="shared" ca="1" si="3"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
+        <f t="shared" si="2"/>
+        <v>45372</v>
+      </c>
+      <c r="B50" t="s">
+        <v>8</v>
+      </c>
+      <c r="C50">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E50">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
+        <f t="shared" si="2"/>
+        <v>45373</v>
+      </c>
+      <c r="B51" t="s">
+        <v>9</v>
+      </c>
+      <c r="C51">
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="D51">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E51">
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
+        <f t="shared" si="2"/>
+        <v>45376</v>
+      </c>
+      <c r="B52" t="s">
+        <v>10</v>
+      </c>
+      <c r="C52">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="D52">
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="E52">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
+        <f t="shared" si="2"/>
+        <v>45378</v>
+      </c>
+      <c r="B53" t="s">
+        <v>11</v>
+      </c>
+      <c r="C53">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="E53">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
+        <f t="shared" si="2"/>
+        <v>45379</v>
+      </c>
+      <c r="B54" t="s">
+        <v>12</v>
+      </c>
+      <c r="C54">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="D54">
+        <f t="shared" ca="1" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="E54">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" s="1">
+        <f t="shared" si="2"/>
+        <v>45380</v>
+      </c>
+      <c r="B55" t="s">
+        <v>13</v>
+      </c>
+      <c r="C55">
+        <f t="shared" ca="1" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="D55">
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="E55">
+        <f t="shared" ca="1" si="3"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" s="1">
+        <f t="shared" si="2"/>
+        <v>45383</v>
+      </c>
+      <c r="B56" t="s">
+        <v>5</v>
+      </c>
+      <c r="C56">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="E56">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" s="1">
+        <f t="shared" si="2"/>
+        <v>45384</v>
+      </c>
+      <c r="B57" t="s">
+        <v>6</v>
+      </c>
+      <c r="C57">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="D57">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E57">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" s="1">
+        <f t="shared" si="2"/>
+        <v>45385</v>
+      </c>
+      <c r="B58" t="s">
+        <v>7</v>
+      </c>
+      <c r="C58">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="D58">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="E58">
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" s="1">
+        <f t="shared" si="2"/>
+        <v>45386</v>
+      </c>
+      <c r="B59" t="s">
+        <v>8</v>
+      </c>
+      <c r="C59">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="E59">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" s="1">
+        <f t="shared" si="2"/>
+        <v>45387</v>
+      </c>
+      <c r="B60" t="s">
+        <v>9</v>
+      </c>
+      <c r="C60">
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="D60">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="E60">
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61" s="1">
+        <f t="shared" si="2"/>
+        <v>45390</v>
+      </c>
+      <c r="B61" t="s">
+        <v>10</v>
+      </c>
+      <c r="C61">
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="D61">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E61">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62" s="1">
+        <f t="shared" si="2"/>
+        <v>45392</v>
+      </c>
+      <c r="B62" t="s">
+        <v>11</v>
+      </c>
+      <c r="C62">
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="D62">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E62">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63" s="1">
+        <f t="shared" si="2"/>
+        <v>45393</v>
+      </c>
+      <c r="B63" t="s">
+        <v>12</v>
+      </c>
+      <c r="C63">
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="D63">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="E63">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A64" s="1">
+        <f t="shared" si="2"/>
+        <v>45394</v>
+      </c>
+      <c r="B64" t="s">
+        <v>13</v>
+      </c>
+      <c r="C64">
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="D64">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="E64">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A65" s="1">
+        <f t="shared" si="2"/>
+        <v>45397</v>
+      </c>
+      <c r="B65" t="s">
+        <v>5</v>
+      </c>
+      <c r="C65">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="D65">
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="E65">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A66" s="1">
+        <f t="shared" si="2"/>
+        <v>45398</v>
+      </c>
+      <c r="B66" t="s">
+        <v>6</v>
+      </c>
+      <c r="C66">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="D66">
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="E66">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67" s="1">
+        <f t="shared" si="2"/>
+        <v>45399</v>
+      </c>
+      <c r="B67" t="s">
+        <v>7</v>
+      </c>
+      <c r="C67">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="D67">
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="E67">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A68" s="1">
+        <f t="shared" si="2"/>
+        <v>45400</v>
+      </c>
+      <c r="B68" t="s">
+        <v>8</v>
+      </c>
+      <c r="C68">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="D68">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E68">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A69" s="1">
+        <f t="shared" si="2"/>
+        <v>45401</v>
+      </c>
+      <c r="B69" t="s">
+        <v>9</v>
+      </c>
+      <c r="C69">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="D69">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E69">
+        <f t="shared" ca="1" si="3"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A70" s="1">
+        <f t="shared" si="2"/>
+        <v>45404</v>
+      </c>
+      <c r="B70" t="s">
+        <v>10</v>
+      </c>
+      <c r="C70">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D70">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E70">
+        <f t="shared" ca="1" si="3"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A71" s="1">
+        <f t="shared" si="2"/>
+        <v>45406</v>
+      </c>
+      <c r="B71" t="s">
+        <v>11</v>
+      </c>
+      <c r="C71">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="D71">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="E71">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A72" s="1">
+        <f t="shared" si="2"/>
+        <v>45407</v>
+      </c>
+      <c r="B72" t="s">
+        <v>12</v>
+      </c>
+      <c r="C72">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="D72">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="E72">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A73" s="1">
+        <f t="shared" si="2"/>
+        <v>45408</v>
+      </c>
+      <c r="B73" t="s">
+        <v>13</v>
+      </c>
+      <c r="C73">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="D73">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="E73">
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A74" s="1">
+        <f t="shared" si="2"/>
+        <v>45411</v>
+      </c>
+      <c r="B74" t="s">
+        <v>5</v>
+      </c>
+      <c r="C74">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D74">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="E74">
+        <f t="shared" ca="1" si="3"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A75" s="1">
+        <f t="shared" si="2"/>
+        <v>45412</v>
+      </c>
+      <c r="B75" t="s">
+        <v>6</v>
+      </c>
+      <c r="C75">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D75">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="E75">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A76" s="1">
+        <f t="shared" ref="A76:A91" si="4">A67+14</f>
+        <v>45413</v>
+      </c>
+      <c r="B76" t="s">
+        <v>7</v>
+      </c>
+      <c r="C76">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D76">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="E76">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A77" s="1">
+        <f t="shared" si="4"/>
+        <v>45414</v>
+      </c>
+      <c r="B77" t="s">
+        <v>8</v>
+      </c>
+      <c r="C77">
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="D77">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="E77">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A78" s="1">
+        <f t="shared" si="4"/>
+        <v>45415</v>
+      </c>
+      <c r="B78" t="s">
+        <v>9</v>
+      </c>
+      <c r="C78">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="D78">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E78">
+        <f t="shared" ca="1" si="3"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A79" s="1">
+        <f t="shared" si="4"/>
+        <v>45418</v>
+      </c>
+      <c r="B79" t="s">
+        <v>10</v>
+      </c>
+      <c r="C79">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="D79">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E79">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A80" s="1">
+        <f t="shared" si="4"/>
+        <v>45420</v>
+      </c>
+      <c r="B80" t="s">
+        <v>11</v>
+      </c>
+      <c r="C80">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="D80">
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="E80">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A81" s="1">
+        <f t="shared" si="4"/>
+        <v>45421</v>
+      </c>
+      <c r="B81" t="s">
+        <v>12</v>
+      </c>
+      <c r="C81">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="D81">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E81">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A82" s="1">
+        <f t="shared" si="4"/>
+        <v>45422</v>
+      </c>
+      <c r="B82" t="s">
+        <v>13</v>
+      </c>
+      <c r="C82">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D82">
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="E82">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A83" s="1">
+        <f t="shared" si="4"/>
+        <v>45425</v>
+      </c>
+      <c r="B83" t="s">
+        <v>5</v>
+      </c>
+      <c r="C83">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D83">
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="E83">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A84" s="1">
+        <f t="shared" si="4"/>
+        <v>45426</v>
+      </c>
+      <c r="B84" t="s">
+        <v>6</v>
+      </c>
+      <c r="C84">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="D84">
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="E84">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A85" s="1">
+        <f t="shared" si="4"/>
+        <v>45427</v>
+      </c>
+      <c r="B85" t="s">
+        <v>7</v>
+      </c>
+      <c r="C85">
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="D85">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="E85">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A86" s="1">
+        <f t="shared" si="4"/>
+        <v>45428</v>
+      </c>
+      <c r="B86" t="s">
+        <v>8</v>
+      </c>
+      <c r="C86">
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="D86">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E86">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A87" s="1">
+        <f t="shared" si="4"/>
+        <v>45429</v>
+      </c>
+      <c r="B87" t="s">
+        <v>9</v>
+      </c>
+      <c r="C87">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D87">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="E87">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A88" s="1">
+        <f t="shared" si="4"/>
+        <v>45432</v>
+      </c>
+      <c r="B88" t="s">
+        <v>10</v>
+      </c>
+      <c r="C88">
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="D88">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E88">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A89" s="1">
+        <f t="shared" si="4"/>
+        <v>45434</v>
+      </c>
+      <c r="B89" t="s">
+        <v>11</v>
+      </c>
+      <c r="C89">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D89">
+        <f t="shared" ca="1" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="E89">
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A90" s="1">
+        <f t="shared" si="4"/>
+        <v>45435</v>
+      </c>
+      <c r="B90" t="s">
+        <v>12</v>
+      </c>
+      <c r="C90">
+        <f t="shared" ca="1" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="D90">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="E90">
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A91" s="1">
+        <f t="shared" si="4"/>
+        <v>45436</v>
+      </c>
+      <c r="B91" t="s">
+        <v>13</v>
+      </c>
+      <c r="C91">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D91">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E91">
+        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
     </row>

</xml_diff>